<commit_message>
Revisión de necesidades y procesos, casos de uso
</commit_message>
<xml_diff>
--- a/01-soft-dev-project/Identificacion_Necesidades_Procesos.xlsx
+++ b/01-soft-dev-project/Identificacion_Necesidades_Procesos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mauricio\Documents\OAUCPN Data\ANT-DPP_ARCGES\01-Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arco-OAUCPN-2024\01-soft-dev-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED03C8F-F794-476E-AE36-DA6DA03F91A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB66901B-1A28-4EC2-8413-F485A98218A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NECESIDADES" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
   <si>
     <t>Lista de necesidades</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Se necesita generar los informes con base en la información recabada de las solicitudes de fichas, clasificando a éstos por tipo de trámite y categoría de licencia.</t>
   </si>
   <si>
-    <t>Se necesita procesar el inventario del archivo de gestión a través de un módulo que refleje lo físico recibido desde los digitadores versus lo lógico que emite AXIS, una vez que se ha finalizado una jornada de trabajo.</t>
-  </si>
-  <si>
     <t>Los procesos de emisión y registro de actas de entrega recepción son manuales y tienden a la introducción de errores generando información no confiable. Se necesita procesos automáticos generados a partir de la información del repositorio de AXIS.</t>
   </si>
   <si>
@@ -208,18 +205,6 @@
   </si>
   <si>
     <t>PROC.01.09</t>
-  </si>
-  <si>
-    <t>Emisión de reportes de transferencia de documentación primaria</t>
-  </si>
-  <si>
-    <t>Gestión de Reportes de Inventario Documental</t>
-  </si>
-  <si>
-    <t>Consolidación de información verificada generadas mediante reportes con base legal, antecedentes, etc., etc.</t>
-  </si>
-  <si>
-    <t>Usuario con rol administrador, jefe o técnico.</t>
   </si>
   <si>
     <t>PROC.01.07
@@ -241,6 +226,36 @@
   </si>
   <si>
     <t>Necesidades Generales del sistema de archivo de gestión ARCO</t>
+  </si>
+  <si>
+    <t>Se necesita procesar el inventario del archivo de gestión a través de un módulo que refleje lo físico recibido desde los digitadores versus lo lógico que emite AXIS, una vez que se ha finalizado una jornada de trabajo, mediante la emisión de actas de actas de entrega - recepción</t>
+  </si>
+  <si>
+    <t>NEC.06</t>
+  </si>
+  <si>
+    <t>Es necesario la ejecución de un control del inventario físico de los expedientes, a través de un componente de software que permita ubicar los expedientes por año, digitador y caja repositoria; todo esto con base en la recopilación de la información regada que se tiene en archivos de Excel y en los repositorios físicos sin ordenar.</t>
+  </si>
+  <si>
+    <t>Consolidación de información verificada y generación de informes técnicos para activación de licencias en la DTICs mediante reportes con base legal, antecedentes, etc., firmados electrónicamente</t>
+  </si>
+  <si>
+    <t>Gestión de Inventario Documental</t>
+  </si>
+  <si>
+    <t>Procesos de gestión de registro de expedientes con los detalles normados en cuanto a requerimientos, actualización, eliminación de éstos. Emisión de reportes de transferencia de documentación primaria en concordancia con la normativa legal y vigente y conexa de la materia, con firma electrónica de los responsables.</t>
+  </si>
+  <si>
+    <t>Usuario con rol jefe o técnico.</t>
+  </si>
+  <si>
+    <t>Usuario con rol técnico.</t>
+  </si>
+  <si>
+    <t>Usuario con rol técnico o digitador.</t>
+  </si>
+  <si>
+    <t>Usuario con rol administrador, jefe.</t>
   </si>
 </sst>
 </file>
@@ -340,7 +355,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -723,11 +738,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -849,6 +903,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1133,10 +1196,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:D10"/>
+  <dimension ref="B1:D11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D2"/>
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,7 +1212,7 @@
     <row r="1" spans="2:4" ht="129.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="33" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C2" s="34"/>
       <c r="D2" s="35"/>
@@ -1189,10 +1252,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="57" x14ac:dyDescent="0.25">
@@ -1203,7 +1266,7 @@
         <v>40</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="42.75" x14ac:dyDescent="0.25">
@@ -1214,18 +1277,29 @@
         <v>41</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="72" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="20" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="44" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1246,8 +1320,8 @@
   </sheetPr>
   <dimension ref="B1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1298,10 +1372,10 @@
         <v>15</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E6" s="26"/>
     </row>
@@ -1327,10 +1401,10 @@
         <v>38</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
@@ -1338,13 +1412,13 @@
         <v>19</v>
       </c>
       <c r="C9" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="28" t="s">
-        <v>47</v>
-      </c>
       <c r="E9" s="29" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="28.5" x14ac:dyDescent="0.2">
@@ -1352,13 +1426,13 @@
         <v>20</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
@@ -1366,13 +1440,13 @@
         <v>21</v>
       </c>
       <c r="C11" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="28" t="s">
-        <v>50</v>
-      </c>
       <c r="E11" s="29" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="28.5" x14ac:dyDescent="0.2">
@@ -1380,55 +1454,55 @@
         <v>22</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B13" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="28" t="s">
+      <c r="E13" s="29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B14" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="29" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B14" s="27" t="s">
+      <c r="D14" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="72" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="29" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="30" t="s">
-        <v>58</v>
-      </c>
       <c r="C15" s="31" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="15.75" hidden="1" x14ac:dyDescent="0.2">

</xml_diff>